<commit_message>
Add lanyard and diffuser to BOM
</commit_message>
<xml_diff>
--- a/Documentation/BOM Core 64 v0.3.0 Dual Boards.xlsx
+++ b/Documentation/BOM Core 64 v0.3.0 Dual Boards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c02d23ac1278198/00_MBP2011-Documents/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{97C7AE3C-CD90-0847-A5D2-29BC7B91D5F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6C421DA7-6891-AC47-820B-149C100BED67}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{97C7AE3C-CD90-0847-A5D2-29BC7B91D5F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DAA7ABF0-EA68-8841-9186-A852B596C82E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30580" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dual Boards" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="171">
   <si>
     <t>Digi-Key Part Number</t>
   </si>
@@ -537,6 +537,12 @@
   </si>
   <si>
     <t>Sticker</t>
+  </si>
+  <si>
+    <t>Lanyard, double ended</t>
+  </si>
+  <si>
+    <t>LED Diffuser</t>
   </si>
 </sst>
 </file>
@@ -555,6 +561,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -564,6 +571,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -661,7 +669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -696,6 +704,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1011,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q57"/>
+  <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33:Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1064,26 +1073,26 @@
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="8">
-        <f>H55/F8</f>
-        <v>86.663366666666661</v>
+        <f>H57/F8</f>
+        <v>87.713366666666673</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="7"/>
       <c r="J7" s="8">
-        <f>K55/I8</f>
-        <v>82.213366666666673</v>
+        <f>K57/I8</f>
+        <v>83.26336666666667</v>
       </c>
       <c r="K7" s="8"/>
       <c r="L7" s="7"/>
       <c r="M7" s="8">
-        <f>N55/L8</f>
-        <v>59.070966666666671</v>
+        <f>N57/L8</f>
+        <v>59.870966666666675</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="7"/>
       <c r="P7" s="8">
-        <f>Q55/O8</f>
-        <v>51.337996666666669</v>
+        <f>Q57/O8</f>
+        <v>51.887996666666666</v>
       </c>
       <c r="Q7" s="9"/>
     </row>
@@ -1247,40 +1256,40 @@
         <v>15</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" ref="H12:H44" si="0">F$8*F12*G12</f>
+        <f t="shared" ref="H12:H46" si="0">F$8*F12*G12</f>
         <v>0.79969999999999997</v>
       </c>
       <c r="I12">
-        <f t="shared" ref="I12:I49" si="1">F12</f>
+        <f t="shared" ref="I12:I51" si="1">F12</f>
         <v>11</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" ref="K12:K44" si="2">I$8*I12*J12</f>
+        <f t="shared" ref="K12:K46" si="2">I$8*I12*J12</f>
         <v>7.9969999999999999</v>
       </c>
       <c r="L12">
-        <f t="shared" ref="L12:L49" si="3">I12</f>
+        <f t="shared" ref="L12:L51" si="3">I12</f>
         <v>11</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="N12" s="1">
-        <f t="shared" ref="N12:N44" si="4">L$8*L12*M12</f>
+        <f t="shared" ref="N12:N46" si="4">L$8*L12*M12</f>
         <v>33.539000000000001</v>
       </c>
       <c r="O12">
-        <f t="shared" ref="O12:O49" si="5">L12</f>
+        <f t="shared" ref="O12:O51" si="5">L12</f>
         <v>11</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="Q12" s="1">
-        <f t="shared" ref="Q12:Q44" si="6">O$8*O12*P12</f>
+        <f t="shared" ref="Q12:Q46" si="6">O$8*O12*P12</f>
         <v>335.39</v>
       </c>
     </row>
@@ -2375,8 +2384,8 @@
     </row>
     <row r="33" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="2"/>
-      <c r="E33" s="2" t="s">
-        <v>146</v>
+      <c r="E33" s="26" t="s">
+        <v>170</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -2385,47 +2394,47 @@
         <v>0.05</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H33" si="7">F$8*F33*G33</f>
         <v>0.05</v>
       </c>
       <c r="I33">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I33" si="8">F33</f>
         <v>1</v>
       </c>
       <c r="J33" s="1">
         <v>0.05</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="K33" si="9">I$8*I33*J33</f>
         <v>0.5</v>
       </c>
       <c r="L33">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="L33" si="10">I33</f>
         <v>1</v>
       </c>
       <c r="M33" s="1">
         <v>0.05</v>
       </c>
       <c r="N33" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="N33" si="11">L$8*L33*M33</f>
         <v>5</v>
       </c>
       <c r="O33">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="O33" si="12">L33</f>
         <v>1</v>
       </c>
       <c r="P33" s="1">
         <v>0.05</v>
       </c>
       <c r="Q33" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="Q33" si="13">O$8*O33*P33</f>
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="2"/>
-      <c r="E34" s="2" t="s">
-        <v>147</v>
+      <c r="E34" t="s">
+        <v>169</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -2434,909 +2443,1007 @@
         <v>1</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H34" si="14">F$8*F34*G34</f>
         <v>1</v>
       </c>
       <c r="I34">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I34" si="15">F34</f>
         <v>1</v>
       </c>
       <c r="J34" s="1">
+        <v>1</v>
+      </c>
+      <c r="K34" s="1">
+        <f t="shared" ref="K34" si="16">I$8*I34*J34</f>
+        <v>10</v>
+      </c>
+      <c r="L34">
+        <f t="shared" ref="L34" si="17">I34</f>
+        <v>1</v>
+      </c>
+      <c r="M34" s="1">
         <v>0.75</v>
       </c>
-      <c r="K34" s="1">
-        <f t="shared" si="2"/>
-        <v>7.5</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M34" s="1">
+      <c r="N34" s="1">
+        <f t="shared" ref="N34" si="18">L$8*L34*M34</f>
+        <v>75</v>
+      </c>
+      <c r="O34">
+        <f t="shared" ref="O34" si="19">L34</f>
+        <v>1</v>
+      </c>
+      <c r="P34" s="1">
         <v>0.5</v>
       </c>
-      <c r="N34" s="1">
-        <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="O34">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="P34" s="1">
-        <v>0.25</v>
-      </c>
       <c r="Q34" s="1">
-        <f t="shared" si="6"/>
-        <v>250</v>
+        <f t="shared" ref="Q34" si="20">O$8*O34*P34</f>
+        <v>500</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="G35" s="15"/>
-      <c r="J35" s="4"/>
+        <v>146</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" s="16">
+        <v>0.05</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J35" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K35" s="1">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="L35">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M35" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="N35" s="1">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P35" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="Q35" s="1">
+        <f t="shared" si="6"/>
+        <v>50</v>
+      </c>
     </row>
     <row r="36" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B36" t="s">
-        <v>157</v>
-      </c>
-      <c r="C36" t="s">
-        <v>158</v>
-      </c>
-      <c r="E36" t="s">
-        <v>154</v>
+      <c r="B36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="F36">
         <v>1</v>
       </c>
-      <c r="G36" s="14">
-        <v>2.41</v>
+      <c r="G36" s="17">
+        <v>1</v>
       </c>
       <c r="H36" s="1">
         <f t="shared" si="0"/>
-        <v>2.41</v>
+        <v>1</v>
       </c>
       <c r="I36">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J36" s="1">
-        <v>2.41</v>
+        <v>0.75</v>
       </c>
       <c r="K36" s="1">
         <f t="shared" si="2"/>
-        <v>24.1</v>
+        <v>7.5</v>
       </c>
       <c r="L36">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M36" s="1">
-        <v>2.14</v>
+        <v>0.5</v>
       </c>
       <c r="N36" s="1">
         <f t="shared" si="4"/>
-        <v>214</v>
+        <v>50</v>
       </c>
       <c r="O36">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="P36" s="1">
-        <v>1.27</v>
+        <v>0.25</v>
       </c>
       <c r="Q36" s="1">
         <f t="shared" si="6"/>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G37" s="15"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B38" t="s">
+        <v>157</v>
+      </c>
+      <c r="C38" t="s">
+        <v>158</v>
+      </c>
+      <c r="E38" t="s">
+        <v>154</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38" s="14">
+        <v>2.41</v>
+      </c>
+      <c r="H38" s="1">
+        <f t="shared" si="0"/>
+        <v>2.41</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J38" s="1">
+        <v>2.41</v>
+      </c>
+      <c r="K38" s="1">
+        <f t="shared" si="2"/>
+        <v>24.1</v>
+      </c>
+      <c r="L38">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M38" s="1">
+        <v>2.14</v>
+      </c>
+      <c r="N38" s="1">
+        <f t="shared" si="4"/>
+        <v>214</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="P38" s="1">
+        <v>1.27</v>
+      </c>
+      <c r="Q38" s="1">
+        <f t="shared" si="6"/>
         <v>1270</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E37" t="s">
+    <row r="39" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E39" t="s">
         <v>137</v>
       </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-      <c r="G37" s="18">
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39" s="18">
         <v>11.65</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H39" s="1">
         <f t="shared" si="0"/>
         <v>11.65</v>
       </c>
-      <c r="I37">
+      <c r="I39">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J39" s="4">
         <v>11.65</v>
       </c>
-      <c r="K37" s="1">
+      <c r="K39" s="1">
         <f t="shared" si="2"/>
         <v>116.5</v>
       </c>
-      <c r="L37">
+      <c r="L39">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M37" s="1">
+      <c r="M39" s="1">
         <v>10</v>
       </c>
-      <c r="N37" s="1">
+      <c r="N39" s="1">
         <f t="shared" si="4"/>
         <v>1000</v>
       </c>
-      <c r="O37">
+      <c r="O39">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P37" s="1">
+      <c r="P39" s="1">
         <v>8</v>
       </c>
-      <c r="Q37" s="1">
+      <c r="Q39" s="1">
         <f t="shared" si="6"/>
         <v>8000</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E38" t="s">
-        <v>163</v>
-      </c>
-      <c r="F38" s="23">
-        <v>2</v>
-      </c>
-      <c r="G38" s="14">
-        <v>2.08</v>
-      </c>
-      <c r="H38" s="24">
-        <f t="shared" ref="H38" si="7">F$8*F38*G38</f>
-        <v>4.16</v>
-      </c>
-      <c r="I38" s="23">
-        <f t="shared" ref="I38" si="8">F38</f>
-        <v>2</v>
-      </c>
-      <c r="J38" s="14">
-        <v>2.08</v>
-      </c>
-      <c r="K38" s="24">
-        <f t="shared" ref="K38" si="9">I$8*I38*J38</f>
-        <v>41.6</v>
-      </c>
-      <c r="L38" s="23">
-        <f t="shared" ref="L38" si="10">I38</f>
-        <v>2</v>
-      </c>
-      <c r="M38" s="24">
-        <v>1.5</v>
-      </c>
-      <c r="N38" s="24">
-        <f t="shared" ref="N38" si="11">L$8*L38*M38</f>
-        <v>300</v>
-      </c>
-      <c r="O38" s="23">
-        <f t="shared" ref="O38" si="12">L38</f>
-        <v>2</v>
-      </c>
-      <c r="P38" s="24">
-        <v>1.5</v>
-      </c>
-      <c r="Q38" s="24">
-        <f t="shared" ref="Q38" si="13">O$8*O38*P38</f>
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E39" t="s">
-        <v>164</v>
-      </c>
-      <c r="F39" s="23">
-        <v>2</v>
-      </c>
-      <c r="G39" s="14">
-        <v>3.65</v>
-      </c>
-      <c r="H39" s="24">
-        <f t="shared" ref="H39" si="14">F$8*F39*G39</f>
-        <v>7.3</v>
-      </c>
-      <c r="I39" s="23">
-        <f t="shared" ref="I39" si="15">F39</f>
-        <v>2</v>
-      </c>
-      <c r="J39" s="14">
-        <v>2.08</v>
-      </c>
-      <c r="K39" s="24">
-        <f t="shared" ref="K39" si="16">I$8*I39*J39</f>
-        <v>41.6</v>
-      </c>
-      <c r="L39" s="23">
-        <f t="shared" ref="L39" si="17">I39</f>
-        <v>2</v>
-      </c>
-      <c r="M39" s="24">
-        <v>2.58</v>
-      </c>
-      <c r="N39" s="24">
-        <f t="shared" ref="N39" si="18">L$8*L39*M39</f>
-        <v>516</v>
-      </c>
-      <c r="O39" s="23">
-        <f t="shared" ref="O39" si="19">L39</f>
-        <v>2</v>
-      </c>
-      <c r="P39" s="24">
-        <v>2.58</v>
-      </c>
-      <c r="Q39" s="24">
-        <f t="shared" ref="Q39" si="20">O$8*O39*P39</f>
-        <v>5160</v>
-      </c>
-    </row>
     <row r="40" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E40" t="s">
+        <v>163</v>
+      </c>
+      <c r="F40" s="23">
+        <v>2</v>
+      </c>
+      <c r="G40" s="14">
+        <v>2.08</v>
+      </c>
+      <c r="H40" s="24">
+        <f t="shared" ref="H40" si="21">F$8*F40*G40</f>
+        <v>4.16</v>
+      </c>
+      <c r="I40" s="23">
+        <f t="shared" ref="I40" si="22">F40</f>
+        <v>2</v>
+      </c>
+      <c r="J40" s="14">
+        <v>2.08</v>
+      </c>
+      <c r="K40" s="24">
+        <f t="shared" ref="K40" si="23">I$8*I40*J40</f>
+        <v>41.6</v>
+      </c>
+      <c r="L40" s="23">
+        <f t="shared" ref="L40" si="24">I40</f>
+        <v>2</v>
+      </c>
+      <c r="M40" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="N40" s="24">
+        <f t="shared" ref="N40" si="25">L$8*L40*M40</f>
+        <v>300</v>
+      </c>
+      <c r="O40" s="23">
+        <f t="shared" ref="O40" si="26">L40</f>
+        <v>2</v>
+      </c>
+      <c r="P40" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="Q40" s="24">
+        <f t="shared" ref="Q40" si="27">O$8*O40*P40</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E41" t="s">
+        <v>164</v>
+      </c>
+      <c r="F41" s="23">
+        <v>2</v>
+      </c>
+      <c r="G41" s="14">
+        <v>3.65</v>
+      </c>
+      <c r="H41" s="24">
+        <f t="shared" ref="H41" si="28">F$8*F41*G41</f>
+        <v>7.3</v>
+      </c>
+      <c r="I41" s="23">
+        <f t="shared" ref="I41" si="29">F41</f>
+        <v>2</v>
+      </c>
+      <c r="J41" s="14">
+        <v>2.08</v>
+      </c>
+      <c r="K41" s="24">
+        <f t="shared" ref="K41" si="30">I$8*I41*J41</f>
+        <v>41.6</v>
+      </c>
+      <c r="L41" s="23">
+        <f t="shared" ref="L41" si="31">I41</f>
+        <v>2</v>
+      </c>
+      <c r="M41" s="24">
+        <v>2.58</v>
+      </c>
+      <c r="N41" s="24">
+        <f t="shared" ref="N41" si="32">L$8*L41*M41</f>
+        <v>516</v>
+      </c>
+      <c r="O41" s="23">
+        <f t="shared" ref="O41" si="33">L41</f>
+        <v>2</v>
+      </c>
+      <c r="P41" s="24">
+        <v>2.58</v>
+      </c>
+      <c r="Q41" s="24">
+        <f t="shared" ref="Q41" si="34">O$8*O41*P41</f>
+        <v>5160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E42" t="s">
         <v>138</v>
       </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-      <c r="G40" s="17">
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42" s="17">
         <v>26.14</v>
       </c>
-      <c r="H40" s="1">
+      <c r="H42" s="1">
         <v>27.2</v>
       </c>
-      <c r="I40">
+      <c r="I42">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J40" s="1">
+      <c r="J42" s="1">
         <v>26.14</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K42" s="1">
         <f t="shared" si="2"/>
         <v>261.39999999999998</v>
       </c>
-      <c r="L40">
+      <c r="L42">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M40" s="1">
+      <c r="M42" s="1">
         <v>16</v>
       </c>
-      <c r="N40" s="1">
+      <c r="N42" s="1">
         <f t="shared" si="4"/>
         <v>1600</v>
       </c>
-      <c r="O40">
+      <c r="O42">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P40" s="1">
+      <c r="P42" s="1">
         <v>16</v>
       </c>
-      <c r="Q40" s="1">
+      <c r="Q42" s="1">
         <f t="shared" si="6"/>
         <v>16000</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E41" t="s">
+    <row r="43" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E43" t="s">
         <v>139</v>
       </c>
-      <c r="F41">
-        <v>1</v>
-      </c>
-      <c r="G41" s="17">
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43" s="17">
         <v>5</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H43" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I41">
+      <c r="I43">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J41" s="1">
+      <c r="J43" s="1">
         <v>5</v>
       </c>
-      <c r="K41" s="1">
+      <c r="K43" s="1">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="L41">
+      <c r="L43">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M41" s="1">
+      <c r="M43" s="1">
         <v>4</v>
       </c>
-      <c r="N41" s="1">
+      <c r="N43" s="1">
         <f t="shared" si="4"/>
         <v>400</v>
       </c>
-      <c r="O41">
+      <c r="O43">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P41" s="1">
+      <c r="P43" s="1">
         <v>3</v>
       </c>
-      <c r="Q41" s="1">
+      <c r="Q43" s="1">
         <f t="shared" si="6"/>
         <v>3000</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E42" t="s">
+    <row r="44" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E44" t="s">
         <v>159</v>
       </c>
-      <c r="F42" s="23">
+      <c r="F44" s="23">
         <v>2</v>
       </c>
-      <c r="G42" s="14">
+      <c r="G44" s="14">
         <v>2.5499999999999998</v>
       </c>
-      <c r="H42" s="24">
-        <f t="shared" ref="H42" si="21">F$8*F42*G42</f>
+      <c r="H44" s="24">
+        <f t="shared" ref="H44" si="35">F$8*F44*G44</f>
         <v>5.0999999999999996</v>
       </c>
-      <c r="I42" s="23">
+      <c r="I44" s="23">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J42" s="24">
+      <c r="J44" s="24">
         <v>2.5499999999999998</v>
       </c>
-      <c r="K42" s="24">
+      <c r="K44" s="24">
         <f t="shared" si="2"/>
         <v>51</v>
       </c>
-      <c r="L42" s="23">
+      <c r="L44" s="23">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M42" s="24">
+      <c r="M44" s="24">
         <v>1.85</v>
       </c>
-      <c r="N42" s="24">
+      <c r="N44" s="24">
         <f t="shared" si="4"/>
         <v>370</v>
       </c>
-      <c r="O42" s="23">
+      <c r="O44" s="23">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="P42" s="25">
+      <c r="P44" s="25">
         <v>1.85</v>
       </c>
-      <c r="Q42" s="24">
+      <c r="Q44" s="24">
         <f t="shared" si="6"/>
         <v>3700</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E43" s="2" t="s">
+    <row r="45" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E45" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="F43" s="23">
+      <c r="F45" s="23">
         <v>2</v>
       </c>
-      <c r="G43" s="14">
+      <c r="G45" s="14">
         <v>2.08</v>
       </c>
-      <c r="H43" s="24">
-        <f t="shared" ref="H43" si="22">F$8*F43*G43</f>
+      <c r="H45" s="24">
+        <f t="shared" ref="H45" si="36">F$8*F45*G45</f>
         <v>4.16</v>
       </c>
-      <c r="I43" s="23">
-        <f t="shared" ref="I43" si="23">F43</f>
+      <c r="I45" s="23">
+        <f t="shared" ref="I45" si="37">F45</f>
         <v>2</v>
       </c>
-      <c r="J43" s="24">
+      <c r="J45" s="24">
         <v>2.08</v>
       </c>
-      <c r="K43" s="24">
-        <f t="shared" ref="K43" si="24">I$8*I43*J43</f>
+      <c r="K45" s="24">
+        <f t="shared" ref="K45" si="38">I$8*I45*J45</f>
         <v>41.6</v>
       </c>
-      <c r="L43" s="23">
-        <f t="shared" ref="L43" si="25">I43</f>
+      <c r="L45" s="23">
+        <f t="shared" ref="L45" si="39">I45</f>
         <v>2</v>
       </c>
-      <c r="M43" s="24">
+      <c r="M45" s="24">
         <v>1.85</v>
       </c>
-      <c r="N43" s="24">
-        <f t="shared" ref="N43" si="26">L$8*L43*M43</f>
+      <c r="N45" s="24">
+        <f t="shared" ref="N45" si="40">L$8*L45*M45</f>
         <v>370</v>
       </c>
-      <c r="O43" s="23">
-        <f t="shared" ref="O43" si="27">L43</f>
+      <c r="O45" s="23">
+        <f t="shared" ref="O45" si="41">L45</f>
         <v>2</v>
       </c>
-      <c r="P43" s="25">
+      <c r="P45" s="25">
         <v>1.85</v>
       </c>
-      <c r="Q43" s="24">
-        <f t="shared" ref="Q43" si="28">O$8*O43*P43</f>
+      <c r="Q45" s="24">
+        <f t="shared" ref="Q45" si="42">O$8*O45*P45</f>
         <v>3700</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C44" t="s">
+    <row r="46" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C46" t="s">
         <v>165</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F44">
-        <v>1</v>
-      </c>
-      <c r="G44" s="1">
+      <c r="F46">
+        <v>1</v>
+      </c>
+      <c r="G46" s="1">
         <v>2</v>
       </c>
-      <c r="H44" s="1">
+      <c r="H46" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I44">
+      <c r="I46">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J44" s="1">
+      <c r="J46" s="1">
         <v>2</v>
       </c>
-      <c r="K44" s="1">
+      <c r="K46" s="1">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="L44">
+      <c r="L46">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M44" s="1">
-        <v>1</v>
-      </c>
-      <c r="N44" s="1">
+      <c r="M46" s="1">
+        <v>1</v>
+      </c>
+      <c r="N46" s="1">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="O44">
+      <c r="O46">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P44" s="1">
+      <c r="P46" s="1">
         <v>0.77</v>
       </c>
-      <c r="Q44" s="1">
+      <c r="Q46" s="1">
         <f t="shared" si="6"/>
         <v>770</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E45" s="2"/>
-      <c r="F45" s="22" t="s">
+    <row r="47" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E47" s="2"/>
+      <c r="F47" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="G45" s="16"/>
-      <c r="H45" s="16">
-        <f>SUM(H11:H44)</f>
-        <v>84.201699999999988</v>
-      </c>
-      <c r="I45" s="22"/>
-      <c r="J45" s="16"/>
-      <c r="K45" s="16">
-        <f>SUM(K11:K44)</f>
-        <v>797.51700000000005</v>
-      </c>
-      <c r="L45" s="22"/>
-      <c r="M45" s="16"/>
-      <c r="N45" s="16">
-        <f>SUM(N11:N44)</f>
-        <v>5760.93</v>
-      </c>
-      <c r="O45" s="22"/>
-      <c r="P45" s="16"/>
-      <c r="Q45" s="16">
-        <f>SUM(Q11:Q44)</f>
-        <v>50106.33</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" t="s">
+      <c r="G47" s="16"/>
+      <c r="H47" s="16">
+        <f>SUM(H11:H46)</f>
+        <v>85.2517</v>
+      </c>
+      <c r="I47" s="22"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16">
+        <f>SUM(K11:K46)</f>
+        <v>808.01700000000005</v>
+      </c>
+      <c r="L47" s="22"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="16">
+        <f>SUM(N11:N46)</f>
+        <v>5840.93</v>
+      </c>
+      <c r="O47" s="22"/>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="16">
+        <f>SUM(Q11:Q46)</f>
+        <v>50656.33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
         <v>151</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="19" t="s">
+      <c r="E48" s="2"/>
+      <c r="F48" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20">
-        <f>H45/F8</f>
-        <v>84.201699999999988</v>
-      </c>
-      <c r="I46" s="19"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="20">
-        <f>K45/I8</f>
-        <v>79.7517</v>
-      </c>
-      <c r="L46" s="19"/>
-      <c r="M46" s="20"/>
-      <c r="N46" s="20">
-        <f>N45/L8</f>
-        <v>57.609300000000005</v>
-      </c>
-      <c r="O46" s="19"/>
-      <c r="P46" s="20"/>
-      <c r="Q46" s="20">
-        <f>Q45/O8</f>
-        <v>50.10633</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E47" t="s">
+      <c r="G48" s="20"/>
+      <c r="H48" s="20">
+        <f>H47/F8</f>
+        <v>85.2517</v>
+      </c>
+      <c r="I48" s="19"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="20">
+        <f>K47/I8</f>
+        <v>80.801700000000011</v>
+      </c>
+      <c r="L48" s="19"/>
+      <c r="M48" s="20"/>
+      <c r="N48" s="20">
+        <f>N47/L8</f>
+        <v>58.409300000000002</v>
+      </c>
+      <c r="O48" s="19"/>
+      <c r="P48" s="20"/>
+      <c r="Q48" s="20">
+        <f>Q47/O8</f>
+        <v>50.656330000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E49" t="s">
         <v>140</v>
       </c>
-      <c r="F47">
+      <c r="F49">
         <v>64</v>
       </c>
-      <c r="G47" s="1">
+      <c r="G49" s="1">
         <f>5/1000</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H47" s="1">
-        <f t="shared" ref="H47:H52" si="29">F$8*F47*G47</f>
+      <c r="H49" s="1">
+        <f t="shared" ref="H49:H54" si="43">F$8*F49*G49</f>
         <v>0.32</v>
       </c>
-      <c r="I47">
+      <c r="I49">
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="J47" s="1">
+      <c r="J49" s="1">
         <f>5/1000</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K47" s="1">
-        <f t="shared" ref="K47:K49" si="30">I$8*I47*J47</f>
+      <c r="K49" s="1">
+        <f t="shared" ref="K49:K51" si="44">I$8*I49*J49</f>
         <v>3.2</v>
       </c>
-      <c r="L47">
+      <c r="L49">
         <f t="shared" si="3"/>
         <v>64</v>
       </c>
-      <c r="M47" s="1">
+      <c r="M49" s="1">
         <f>5/1000</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="N47" s="1">
-        <f t="shared" ref="N47:N49" si="31">L$8*L47*M47</f>
+      <c r="N49" s="1">
+        <f t="shared" ref="N49:N51" si="45">L$8*L49*M49</f>
         <v>32</v>
       </c>
-      <c r="O47">
+      <c r="O49">
         <f t="shared" si="5"/>
         <v>64</v>
       </c>
-      <c r="P47" s="1">
+      <c r="P49" s="1">
         <f>5/1000</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="Q47" s="1">
-        <f t="shared" ref="Q47:Q49" si="32">O$8*O47*P47</f>
+      <c r="Q49" s="1">
+        <f t="shared" ref="Q49:Q51" si="46">O$8*O49*P49</f>
         <v>320</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E48" s="2" t="s">
+    <row r="50" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E50" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="F48">
+      <c r="F50">
         <v>70</v>
       </c>
-      <c r="G48" s="5">
+      <c r="G50" s="5">
         <f>10/(1400*12)</f>
         <v>5.9523809523809529E-4</v>
       </c>
-      <c r="H48" s="1">
-        <f t="shared" si="29"/>
+      <c r="H50" s="1">
+        <f t="shared" si="43"/>
         <v>4.1666666666666671E-2</v>
       </c>
-      <c r="I48">
+      <c r="I50">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="J48" s="5">
+      <c r="J50" s="5">
         <f>10/(1400*12)</f>
         <v>5.9523809523809529E-4</v>
       </c>
-      <c r="K48" s="1">
-        <f t="shared" si="30"/>
+      <c r="K50" s="1">
+        <f t="shared" si="44"/>
         <v>0.41666666666666669</v>
       </c>
-      <c r="L48">
+      <c r="L50">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="M48" s="5">
+      <c r="M50" s="5">
         <f>10/(1400*12)</f>
         <v>5.9523809523809529E-4</v>
       </c>
-      <c r="N48" s="1">
-        <f t="shared" si="31"/>
+      <c r="N50" s="1">
+        <f t="shared" si="45"/>
         <v>4.166666666666667</v>
       </c>
-      <c r="O48">
+      <c r="O50">
         <f t="shared" si="5"/>
         <v>70</v>
       </c>
-      <c r="P48" s="5">
+      <c r="P50" s="5">
         <f>10/(1400*12)</f>
         <v>5.9523809523809529E-4</v>
       </c>
-      <c r="Q48" s="1">
-        <f t="shared" si="32"/>
+      <c r="Q50" s="1">
+        <f t="shared" si="46"/>
         <v>41.666666666666671</v>
       </c>
     </row>
-    <row r="49" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C49" t="s">
+    <row r="51" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C51" t="s">
         <v>165</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49" s="1">
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51" s="1">
         <v>2</v>
       </c>
-      <c r="H49" s="1">
-        <f t="shared" si="29"/>
+      <c r="H51" s="1">
+        <f t="shared" si="43"/>
         <v>2</v>
       </c>
-      <c r="I49">
+      <c r="I51">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="J49" s="1">
+      <c r="J51" s="1">
         <v>2</v>
       </c>
-      <c r="K49" s="1">
-        <f t="shared" si="30"/>
+      <c r="K51" s="1">
+        <f t="shared" si="44"/>
         <v>20</v>
       </c>
-      <c r="L49">
+      <c r="L51">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M49" s="1">
-        <v>1</v>
-      </c>
-      <c r="N49" s="1">
-        <f t="shared" si="31"/>
+      <c r="M51" s="1">
+        <v>1</v>
+      </c>
+      <c r="N51" s="1">
+        <f t="shared" si="45"/>
         <v>100</v>
       </c>
-      <c r="O49">
+      <c r="O51">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="P49" s="1">
+      <c r="P51" s="1">
         <v>0.77</v>
       </c>
-      <c r="Q49" s="1">
-        <f t="shared" si="32"/>
+      <c r="Q51" s="1">
+        <f t="shared" si="46"/>
         <v>770</v>
-      </c>
-    </row>
-    <row r="50" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E50" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="51" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E51" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-      <c r="G51" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="H51" s="1">
-        <f t="shared" si="29"/>
-        <v>0.05</v>
-      </c>
-      <c r="I51">
-        <f t="shared" ref="I51:I52" si="33">F51</f>
-        <v>1</v>
-      </c>
-      <c r="J51" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="K51" s="1">
-        <f t="shared" ref="K51:K52" si="34">I$8*I51*J51</f>
-        <v>0.5</v>
-      </c>
-      <c r="L51">
-        <f t="shared" ref="L51:L52" si="35">I51</f>
-        <v>1</v>
-      </c>
-      <c r="M51" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="N51" s="1">
-        <f t="shared" ref="N51:N52" si="36">L$8*L51*M51</f>
-        <v>5</v>
-      </c>
-      <c r="O51">
-        <f t="shared" ref="O51:O52" si="37">L51</f>
-        <v>1</v>
-      </c>
-      <c r="P51" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="Q51" s="1">
-        <f t="shared" ref="Q51:Q52" si="38">O$8*O51*P51</f>
-        <v>50</v>
       </c>
     </row>
     <row r="52" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E52" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="53" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E53" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="H53" s="1">
+        <f t="shared" si="43"/>
+        <v>0.05</v>
+      </c>
+      <c r="I53">
+        <f t="shared" ref="I53:I54" si="47">F53</f>
+        <v>1</v>
+      </c>
+      <c r="J53" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K53" s="1">
+        <f t="shared" ref="K53:K54" si="48">I$8*I53*J53</f>
+        <v>0.5</v>
+      </c>
+      <c r="L53">
+        <f t="shared" ref="L53:L54" si="49">I53</f>
+        <v>1</v>
+      </c>
+      <c r="M53" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="N53" s="1">
+        <f t="shared" ref="N53:N54" si="50">L$8*L53*M53</f>
+        <v>5</v>
+      </c>
+      <c r="O53">
+        <f t="shared" ref="O53:O54" si="51">L53</f>
+        <v>1</v>
+      </c>
+      <c r="P53" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="Q53" s="1">
+        <f t="shared" ref="Q53:Q54" si="52">O$8*O53*P53</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E54" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="F52">
-        <v>1</v>
-      </c>
-      <c r="G52" s="1">
+      <c r="F54">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1">
         <v>0.05</v>
       </c>
-      <c r="H52" s="1">
-        <f t="shared" si="29"/>
+      <c r="H54" s="1">
+        <f t="shared" si="43"/>
         <v>0.05</v>
       </c>
-      <c r="I52">
-        <f t="shared" si="33"/>
-        <v>1</v>
-      </c>
-      <c r="J52" s="1">
+      <c r="I54">
+        <f t="shared" si="47"/>
+        <v>1</v>
+      </c>
+      <c r="J54" s="1">
         <v>0.05</v>
       </c>
-      <c r="K52" s="1">
-        <f t="shared" si="34"/>
+      <c r="K54" s="1">
+        <f t="shared" si="48"/>
         <v>0.5</v>
       </c>
-      <c r="L52">
-        <f t="shared" si="35"/>
-        <v>1</v>
-      </c>
-      <c r="M52" s="1">
+      <c r="L54">
+        <f t="shared" si="49"/>
+        <v>1</v>
+      </c>
+      <c r="M54" s="1">
         <v>0.05</v>
       </c>
-      <c r="N52" s="1">
-        <f t="shared" si="36"/>
+      <c r="N54" s="1">
+        <f t="shared" si="50"/>
         <v>5</v>
       </c>
-      <c r="O52">
-        <f t="shared" si="37"/>
-        <v>1</v>
-      </c>
-      <c r="P52" s="1">
+      <c r="O54">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="P54" s="1">
         <v>0.05</v>
       </c>
-      <c r="Q52" s="1">
-        <f t="shared" si="38"/>
+      <c r="Q54" s="1">
+        <f t="shared" si="52"/>
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E53" s="2"/>
-      <c r="F53" s="22" t="s">
+    <row r="55" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E55" s="2"/>
+      <c r="F55" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="G53" s="16"/>
-      <c r="H53" s="16">
-        <f>SUM(H47:H52)</f>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16">
+        <f>SUM(H49:H54)</f>
         <v>2.4616666666666664</v>
       </c>
-      <c r="I53" s="22"/>
-      <c r="J53" s="16"/>
-      <c r="K53" s="16">
-        <f>SUM(K47:K52)</f>
+      <c r="I55" s="22"/>
+      <c r="J55" s="16"/>
+      <c r="K55" s="16">
+        <f>SUM(K49:K54)</f>
         <v>24.616666666666667</v>
       </c>
-      <c r="L53" s="22"/>
-      <c r="M53" s="16"/>
-      <c r="N53" s="16">
-        <f>SUM(N47:N52)</f>
+      <c r="L55" s="22"/>
+      <c r="M55" s="16"/>
+      <c r="N55" s="16">
+        <f>SUM(N49:N54)</f>
         <v>146.16666666666666</v>
       </c>
-      <c r="O53" s="22"/>
-      <c r="P53" s="16"/>
-      <c r="Q53" s="16">
-        <f>SUM(Q47:Q52)</f>
+      <c r="O55" s="22"/>
+      <c r="P55" s="16"/>
+      <c r="Q55" s="16">
+        <f>SUM(Q49:Q54)</f>
         <v>1231.6666666666667</v>
       </c>
     </row>
-    <row r="54" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E54" s="2"/>
-      <c r="F54" s="19" t="s">
+    <row r="56" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E56" s="2"/>
+      <c r="F56" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20">
-        <f>H53/F8</f>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20">
+        <f>H55/F8</f>
         <v>2.4616666666666664</v>
       </c>
-      <c r="I54" s="19"/>
-      <c r="J54" s="20"/>
-      <c r="K54" s="20">
-        <f>K53/I8</f>
+      <c r="I56" s="19"/>
+      <c r="J56" s="20"/>
+      <c r="K56" s="20">
+        <f>K55/I8</f>
         <v>2.4616666666666669</v>
       </c>
-      <c r="L54" s="19"/>
-      <c r="M54" s="20"/>
-      <c r="N54" s="20">
-        <f>N53/L8</f>
+      <c r="L56" s="19"/>
+      <c r="M56" s="20"/>
+      <c r="N56" s="20">
+        <f>N55/L8</f>
         <v>1.4616666666666667</v>
       </c>
-      <c r="O54" s="19"/>
-      <c r="P54" s="20"/>
-      <c r="Q54" s="20">
-        <f>Q53/O8</f>
+      <c r="O56" s="19"/>
+      <c r="P56" s="20"/>
+      <c r="Q56" s="20">
+        <f>Q55/O8</f>
         <v>1.2316666666666667</v>
       </c>
     </row>
-    <row r="55" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E55" s="3" t="s">
+    <row r="57" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E57" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="H55" s="1">
-        <f>H45+H53</f>
-        <v>86.663366666666661</v>
-      </c>
-      <c r="K55" s="1">
-        <f>K45+K53</f>
-        <v>822.13366666666673</v>
-      </c>
-      <c r="N55" s="1">
-        <f>N45+N53</f>
-        <v>5907.0966666666673</v>
-      </c>
-      <c r="Q55" s="1">
-        <f>Q45+Q53</f>
-        <v>51337.996666666666</v>
-      </c>
-    </row>
-    <row r="56" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E56" s="3"/>
-    </row>
-    <row r="57" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F57" s="21" t="s">
+      <c r="H57" s="1">
+        <f>H47+H55</f>
+        <v>87.713366666666673</v>
+      </c>
+      <c r="K57" s="1">
+        <f>K47+K55</f>
+        <v>832.63366666666673</v>
+      </c>
+      <c r="N57" s="1">
+        <f>N47+N55</f>
+        <v>5987.0966666666673</v>
+      </c>
+      <c r="Q57" s="1">
+        <f>Q47+Q55</f>
+        <v>51887.996666666666</v>
+      </c>
+    </row>
+    <row r="58" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="3:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F59" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="H57" s="1">
-        <f>H55/F8</f>
-        <v>86.663366666666661</v>
-      </c>
-      <c r="K57" s="1">
-        <f>K55/I8</f>
-        <v>82.213366666666673</v>
-      </c>
-      <c r="N57" s="1">
-        <f>N55/L8</f>
-        <v>59.070966666666671</v>
-      </c>
-      <c r="Q57" s="1">
-        <f>Q55/O8</f>
-        <v>51.337996666666669</v>
+      <c r="H59" s="1">
+        <f>H57/F8</f>
+        <v>87.713366666666673</v>
+      </c>
+      <c r="K59" s="1">
+        <f>K57/I8</f>
+        <v>83.26336666666667</v>
+      </c>
+      <c r="N59" s="1">
+        <f>N57/L8</f>
+        <v>59.870966666666675</v>
+      </c>
+      <c r="Q59" s="1">
+        <f>Q57/O8</f>
+        <v>51.887996666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>